<commit_message>
Clean up MD/PhD Interview Invite Analyzer and deleted extra files
</commit_message>
<xml_diff>
--- a/fencer data/fencer_cycle_info.xlsx
+++ b/fencer data/fencer_cycle_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Python Analysis\fencer data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A4192C-EA7A-47FB-93A7-7438FC4DE827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B933CA9-0736-4253-BF67-A9BB0DB351D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{CD2684FF-1585-4EFB-A284-DAE4AEFE2B64}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CD2684FF-1585-4EFB-A284-DAE4AEFE2B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Cycle_2020-2021" sheetId="2" r:id="rId1"/>
@@ -6630,9 +6630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9618D1-8B78-478F-AB82-0C3782384149}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7817,8 +7817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E60403-B5D2-4EA3-8F86-A674DBAB247F}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8220,20 +8220,244 @@
       <c r="A8" t="s">
         <v>77</v>
       </c>
+      <c r="E8">
+        <f>(E6-D6*(D2/E2))/(E10/E2)</f>
+        <v>3.8066666666666666</v>
+      </c>
+      <c r="F8">
+        <f>(F6-E6*(E2/F2))/(F10/F2)</f>
+        <v>3.82</v>
+      </c>
+      <c r="G8">
+        <f>(G6-F6*(F2/G2))/(G10/G2)</f>
+        <v>3.7939999999999996</v>
+      </c>
+      <c r="H8">
+        <f>(H6-G6*(G2/H2))/(H10/H2)</f>
+        <v>3.8517777777777775</v>
+      </c>
+      <c r="I8">
+        <f>(I6-H6*(H2/I2))/(I10/I2)</f>
+        <v>3.82</v>
+      </c>
+      <c r="J8">
+        <f>(J6-I6*(I2/J2))/(J10/J2)</f>
+        <v>3.5560000000000014</v>
+      </c>
+      <c r="K8">
+        <f>(K6-J6*(J2/K2))/(K10/K2)</f>
+        <v>3.92263157894737</v>
+      </c>
+      <c r="M8">
+        <f>(M6-K6*(K2/M2))/(M10/M2)</f>
+        <v>3.787244897959182</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="L8:S8" si="0">(N6-M6*(M2/N2))/(N10/N2)</f>
+        <v>3.8200000000000016</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>3.7584848484848496</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>3.81</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>3.5828124999999966</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000043</v>
+      </c>
+      <c r="S8">
+        <f>(S6-R6*(R2/S2))/(S10/S2)</f>
+        <v>3.6574576271186441</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
+      <c r="E9">
+        <f>(E7-D7*(D2/E2))/(E10/E2)</f>
+        <v>515.59999999999991</v>
+      </c>
+      <c r="F9">
+        <f>(F7-E7*(E2/F2))/(F10/F2)</f>
+        <v>518</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ref="G9:S9" si="1">(G7-F7*(F2/G2))/(G10/G2)</f>
+        <v>517.66000000000008</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>516.2466666666669</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>517.58484848484818</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>512.81200000000024</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>519.77684210526331</v>
+      </c>
+      <c r="M9">
+        <f>(M7-K7*(K2/M2))/(M10/M2)</f>
+        <v>515.29122448979558</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>516.72373626373667</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>516.38484848484836</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>518.51627906976773</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>501.19687499999912</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>513.55636363636518</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="1"/>
+        <v>514.77457627118599</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
+      <c r="E10">
+        <f>E2-D2</f>
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ref="F10:S10" si="2">F2-E2</f>
+        <v>44</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>66</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>57</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>81</v>
+      </c>
+      <c r="M10">
+        <f>M2-K2</f>
+        <v>98</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>99</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>86</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="S10">
+        <f>S2-R2</f>
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
+      </c>
+      <c r="E11">
+        <f>ABS(E4-C4)</f>
+        <v>88</v>
+      </c>
+      <c r="F11">
+        <f>ABS(F4-E4)</f>
+        <v>147</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:S11" si="3">ABS(G4-F4)</f>
+        <v>17</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>228</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <f>ABS(M4-K4)</f>
+        <v>68</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="3"/>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
starting the MD/PhD Acceptance Analyzer
</commit_message>
<xml_diff>
--- a/fencer data/fencer_cycle_info.xlsx
+++ b/fencer data/fencer_cycle_info.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Python Analysis\fencer data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B933CA9-0736-4253-BF67-A9BB0DB351D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22335052-E605-4CF1-B439-7BEE357421E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CD2684FF-1585-4EFB-A284-DAE4AEFE2B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Cycle_2020-2021" sheetId="2" r:id="rId1"/>
     <sheet name="Cycle_2021-2022" sheetId="1" r:id="rId2"/>
-    <sheet name="Cycle_2020-2021 argv" sheetId="3" r:id="rId3"/>
+    <sheet name="Cycle_2021-2022_t" sheetId="4" r:id="rId3"/>
+    <sheet name="Cycle_2020-2021 argv" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="374">
   <si>
     <t>date</t>
   </si>
@@ -1135,13 +1136,88 @@
   </si>
   <si>
     <t>25​</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>GPA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GPA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Δ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MCAT</t>
+    </r>
+  </si>
+  <si>
+    <t>predict_GPA</t>
+  </si>
+  <si>
+    <t>predict_MCAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1157,13 +1233,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1187,7 +1287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1200,6 +1300,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6628,11 +6733,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9618D1-8B78-478F-AB82-0C3782384149}">
-  <dimension ref="A1:T43"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H37" sqref="H37"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7406,10 +7511,10 @@
         <v>1599</v>
       </c>
       <c r="D29">
+        <v>3.71</v>
+      </c>
+      <c r="E29">
         <v>512.29999999999995</v>
-      </c>
-      <c r="E29">
-        <v>3.71</v>
       </c>
       <c r="M29" t="s">
         <v>105</v>
@@ -7435,10 +7540,10 @@
         <v>17</v>
       </c>
       <c r="D30">
+        <v>3.79</v>
+      </c>
+      <c r="E30">
         <v>514.5</v>
-      </c>
-      <c r="E30">
-        <v>3.79</v>
       </c>
       <c r="M30" t="s">
         <v>23</v>
@@ -7466,11 +7571,11 @@
       </c>
       <c r="D31">
         <f>D32*(C32/C31) + D34*(C34/C31)</f>
-        <v>512.50117187499995</v>
+        <v>3.6858007812499998</v>
       </c>
       <c r="E31">
         <f>E32*(C32/C31) + E34*(C34/C31)</f>
-        <v>3.6858007812499998</v>
+        <v>512.50117187499995</v>
       </c>
       <c r="M31" t="s">
         <v>350</v>
@@ -7487,10 +7592,10 @@
         <v>177</v>
       </c>
       <c r="D32">
+        <v>3.64</v>
+      </c>
+      <c r="E32">
         <v>510.8</v>
-      </c>
-      <c r="E32">
-        <v>3.64</v>
       </c>
       <c r="M32" t="s">
         <v>31</v>
@@ -7547,10 +7652,10 @@
         <v>335</v>
       </c>
       <c r="D34">
+        <v>3.71</v>
+      </c>
+      <c r="E34">
         <v>513.4</v>
-      </c>
-      <c r="E34">
-        <v>3.71</v>
       </c>
       <c r="M34" t="s">
         <v>29</v>
@@ -7576,10 +7681,10 @@
         <v>14</v>
       </c>
       <c r="D35">
+        <v>3.91</v>
+      </c>
+      <c r="E35">
         <v>518.4</v>
-      </c>
-      <c r="E35">
-        <v>3.91</v>
       </c>
       <c r="M35" t="s">
         <v>35</v>
@@ -7638,11 +7743,11 @@
       </c>
       <c r="D37">
         <f>D38*(C38/C37) + D39*(C39/C37)</f>
-        <v>513.51957255343086</v>
+        <v>3.750123734533183</v>
       </c>
       <c r="E37">
         <f>E38*(C38/C37) + E39*(C39/C37)</f>
-        <v>3.750123734533183</v>
+        <v>513.51957255343086</v>
       </c>
       <c r="M37" t="s">
         <v>340</v>
@@ -7659,10 +7764,10 @@
         <v>683</v>
       </c>
       <c r="D38">
+        <v>3.72</v>
+      </c>
+      <c r="E38">
         <v>512.5</v>
-      </c>
-      <c r="E38">
-        <v>3.72</v>
       </c>
       <c r="M38" t="s">
         <v>21</v>
@@ -7688,10 +7793,10 @@
         <v>206</v>
       </c>
       <c r="D39">
+        <v>3.85</v>
+      </c>
+      <c r="E39">
         <v>516.9</v>
-      </c>
-      <c r="E39">
-        <v>3.85</v>
       </c>
       <c r="M39" t="s">
         <v>18</v>
@@ -7719,11 +7824,11 @@
       </c>
       <c r="D40">
         <f>D41*(C41/C40) + D42*(C42/C40)</f>
-        <v>503.80059880239526</v>
+        <v>3.5725149700598804</v>
       </c>
       <c r="E40">
         <f>E41*(C41/C40) + E42*(C42/C40)</f>
-        <v>3.5725149700598804</v>
+        <v>503.80059880239526</v>
       </c>
       <c r="M40" t="s">
         <v>337</v>
@@ -7740,10 +7845,10 @@
         <v>142</v>
       </c>
       <c r="D41">
+        <v>3.58</v>
+      </c>
+      <c r="E41">
         <v>504.1</v>
-      </c>
-      <c r="E41">
-        <v>3.58</v>
       </c>
       <c r="M41" t="s">
         <v>25</v>
@@ -7769,10 +7874,10 @@
         <v>25</v>
       </c>
       <c r="D42">
+        <v>3.53</v>
+      </c>
+      <c r="E42">
         <v>502.1</v>
-      </c>
-      <c r="E42">
-        <v>3.53</v>
       </c>
       <c r="M42" t="s">
         <v>27</v>
@@ -7800,12 +7905,57 @@
       </c>
       <c r="D43">
         <f>D37*(C37/C43) + D40*(C40/C43)</f>
-        <v>511.98257575757577</v>
+        <v>3.7220359848484845</v>
       </c>
       <c r="E43">
         <f>E37*(C37/C43) + E40*(C40/C43)</f>
-        <v>3.7220359848484845</v>
-      </c>
+        <v>511.98257575757577</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7814,11 +7964,1711 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2310B4-7AF2-4DAE-BF17-FA18602AB5E2}">
+  <dimension ref="A1:N121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="11">
+        <v>44454</v>
+      </c>
+      <c r="D1" s="11">
+        <v>44470</v>
+      </c>
+      <c r="E1" s="11">
+        <v>44474</v>
+      </c>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>1503</v>
+      </c>
+      <c r="D2">
+        <v>1574</v>
+      </c>
+      <c r="E2">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4">
+        <v>248</v>
+      </c>
+      <c r="D4">
+        <v>497</v>
+      </c>
+      <c r="E4">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>159</v>
+      </c>
+      <c r="D5">
+        <v>169</v>
+      </c>
+      <c r="E5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>89</v>
+      </c>
+      <c r="D7">
+        <v>328</v>
+      </c>
+      <c r="E7">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10">
+        <v>1238</v>
+      </c>
+      <c r="D10">
+        <v>900</v>
+      </c>
+      <c r="E10">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>903</v>
+      </c>
+      <c r="D11">
+        <v>703</v>
+      </c>
+      <c r="E11">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>343</v>
+      </c>
+      <c r="D12">
+        <v>197</v>
+      </c>
+      <c r="E12">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13">
+        <v>163</v>
+      </c>
+      <c r="E13">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14">
+        <v>115</v>
+      </c>
+      <c r="D14">
+        <v>137</v>
+      </c>
+      <c r="E14">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>35</v>
+      </c>
+      <c r="D15">
+        <v>26</v>
+      </c>
+      <c r="E15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C16">
+        <v>1238</v>
+      </c>
+      <c r="D16">
+        <v>1063</v>
+      </c>
+      <c r="E16">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>3.73</v>
+      </c>
+      <c r="D17">
+        <v>3.72</v>
+      </c>
+      <c r="E17">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>3.75</v>
+      </c>
+      <c r="D18">
+        <v>3.83</v>
+      </c>
+      <c r="E18">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19">
+        <v>3.633064516129032</v>
+      </c>
+      <c r="D19">
+        <v>3.6895975855130785</v>
+      </c>
+      <c r="E19">
+        <v>3.6858007812499998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20">
+        <v>3.59</v>
+      </c>
+      <c r="D20">
+        <v>3.65</v>
+      </c>
+      <c r="E20">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B21" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>3.71</v>
+      </c>
+      <c r="D22">
+        <v>3.71</v>
+      </c>
+      <c r="E22">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23">
+        <v>3.98</v>
+      </c>
+      <c r="D23">
+        <v>3.87</v>
+      </c>
+      <c r="E23">
+        <v>3.91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C25">
+        <v>3.7410500807754441</v>
+      </c>
+      <c r="D25">
+        <v>3.7562666666666664</v>
+      </c>
+      <c r="E25">
+        <v>3.750123734533183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>3.74</v>
+      </c>
+      <c r="D26">
+        <v>3.73</v>
+      </c>
+      <c r="E26">
+        <v>3.72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B27" t="s">
+        <v>343</v>
+      </c>
+      <c r="D27">
+        <v>3.85</v>
+      </c>
+      <c r="E27">
+        <v>3.85</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="D28">
+        <v>3.588834355828221</v>
+      </c>
+      <c r="E28">
+        <v>3.5725149700598804</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29">
+        <v>3.64</v>
+      </c>
+      <c r="D29">
+        <v>3.6</v>
+      </c>
+      <c r="E29">
+        <v>3.58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>3.63</v>
+      </c>
+      <c r="D30">
+        <v>3.53</v>
+      </c>
+      <c r="E30">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B31" t="s">
+        <v>344</v>
+      </c>
+      <c r="C31">
+        <v>3.7410500807754441</v>
+      </c>
+      <c r="D31">
+        <v>3.7305926622765755</v>
+      </c>
+      <c r="E31">
+        <v>3.7220359848484845</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32">
+        <v>512.9</v>
+      </c>
+      <c r="D32">
+        <v>512.5</v>
+      </c>
+      <c r="E32">
+        <v>512.29999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33">
+        <v>512.6</v>
+      </c>
+      <c r="D33">
+        <v>515.29999999999995</v>
+      </c>
+      <c r="E33">
+        <v>514.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34">
+        <v>510.64354838709676</v>
+      </c>
+      <c r="D34">
+        <v>512.48189134808854</v>
+      </c>
+      <c r="E34">
+        <v>512.50117187499995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35">
+        <v>510.5</v>
+      </c>
+      <c r="D35">
+        <v>510.7</v>
+      </c>
+      <c r="E35">
+        <v>510.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37">
+        <v>510.9</v>
+      </c>
+      <c r="D37">
+        <v>513.4</v>
+      </c>
+      <c r="E37">
+        <v>513.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
+        <v>132</v>
+      </c>
+      <c r="C38">
+        <v>520.29999999999995</v>
+      </c>
+      <c r="D38">
+        <v>521.5</v>
+      </c>
+      <c r="E38">
+        <v>518.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
+        <v>153</v>
+      </c>
+      <c r="C40">
+        <v>513.29353796445878</v>
+      </c>
+      <c r="D40">
+        <v>513.66311111111122</v>
+      </c>
+      <c r="E40">
+        <v>513.51957255343086</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41">
+        <v>513.79999999999995</v>
+      </c>
+      <c r="D41">
+        <v>512.70000000000005</v>
+      </c>
+      <c r="E41">
+        <v>512.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" t="s">
+        <v>343</v>
+      </c>
+      <c r="D42">
+        <v>517.1</v>
+      </c>
+      <c r="E42">
+        <v>516.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43">
+        <v>504.48098159509203</v>
+      </c>
+      <c r="E43">
+        <v>503.80059880239526</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44">
+        <v>505.8</v>
+      </c>
+      <c r="D44">
+        <v>504.8</v>
+      </c>
+      <c r="E44">
+        <v>504.1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45">
+        <v>504.2</v>
+      </c>
+      <c r="D45">
+        <v>502.8</v>
+      </c>
+      <c r="E45">
+        <v>502.1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" t="s">
+        <v>344</v>
+      </c>
+      <c r="C46">
+        <v>513.29353796445878</v>
+      </c>
+      <c r="D46">
+        <v>512.25512699905937</v>
+      </c>
+      <c r="E46">
+        <v>511.98257575757577</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47" t="e">
+        <f>na</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D47">
+        <f>D2-C2</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="e">
+        <f t="shared" ref="C48:D111" si="0">na</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ref="D48:D61" si="1">D3-C3</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B50" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B51" t="s">
+        <v>267</v>
+      </c>
+      <c r="C51" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D51" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B53" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D54" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B55" t="s">
+        <v>153</v>
+      </c>
+      <c r="C55" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>-338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B57" t="s">
+        <v>343</v>
+      </c>
+      <c r="C57" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D57" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B58" t="s">
+        <v>154</v>
+      </c>
+      <c r="C58" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D58" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B59" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="B61" t="s">
+        <v>344</v>
+      </c>
+      <c r="C61" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>-175</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B63" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B64" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B65" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B66" t="s">
+        <v>267</v>
+      </c>
+      <c r="C66" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B67" t="s">
+        <v>30</v>
+      </c>
+      <c r="C67" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B68" t="s">
+        <v>132</v>
+      </c>
+      <c r="C68" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B70" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B71" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B72" t="s">
+        <v>343</v>
+      </c>
+      <c r="C72" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B73" t="s">
+        <v>154</v>
+      </c>
+      <c r="C73" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B74" t="s">
+        <v>26</v>
+      </c>
+      <c r="C74" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="B76" t="s">
+        <v>344</v>
+      </c>
+      <c r="C76" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B77" t="s">
+        <v>33</v>
+      </c>
+      <c r="C77" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B78" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B79" t="s">
+        <v>104</v>
+      </c>
+      <c r="C79" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B80" t="s">
+        <v>32</v>
+      </c>
+      <c r="C80" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B81" t="s">
+        <v>267</v>
+      </c>
+      <c r="C81" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B82" t="s">
+        <v>30</v>
+      </c>
+      <c r="C82" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B83" t="s">
+        <v>132</v>
+      </c>
+      <c r="C83" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C84" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B85" t="s">
+        <v>153</v>
+      </c>
+      <c r="C85" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B86" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B87" t="s">
+        <v>343</v>
+      </c>
+      <c r="C87" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B88" t="s">
+        <v>154</v>
+      </c>
+      <c r="C88" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B89" t="s">
+        <v>26</v>
+      </c>
+      <c r="C89" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B90" t="s">
+        <v>28</v>
+      </c>
+      <c r="C90" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="B91" t="s">
+        <v>344</v>
+      </c>
+      <c r="C91" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B92" t="s">
+        <v>33</v>
+      </c>
+      <c r="C92" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B93" t="s">
+        <v>34</v>
+      </c>
+      <c r="C93" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B94" t="s">
+        <v>104</v>
+      </c>
+      <c r="C94" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B95" t="s">
+        <v>32</v>
+      </c>
+      <c r="C95" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B96" t="s">
+        <v>267</v>
+      </c>
+      <c r="C96" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B97" t="s">
+        <v>30</v>
+      </c>
+      <c r="C97" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B98" t="s">
+        <v>132</v>
+      </c>
+      <c r="C98" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B99" t="s">
+        <v>37</v>
+      </c>
+      <c r="C99" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B100" t="s">
+        <v>153</v>
+      </c>
+      <c r="C100" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B101" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B102" t="s">
+        <v>343</v>
+      </c>
+      <c r="C102" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B103" t="s">
+        <v>154</v>
+      </c>
+      <c r="C103" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B104" t="s">
+        <v>26</v>
+      </c>
+      <c r="C104" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B105" t="s">
+        <v>28</v>
+      </c>
+      <c r="C105" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B106" t="s">
+        <v>344</v>
+      </c>
+      <c r="C106" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B107" t="s">
+        <v>33</v>
+      </c>
+      <c r="C107" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B108" t="s">
+        <v>34</v>
+      </c>
+      <c r="C108" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B109" t="s">
+        <v>104</v>
+      </c>
+      <c r="C109" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B110" t="s">
+        <v>32</v>
+      </c>
+      <c r="C110" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B111" t="s">
+        <v>267</v>
+      </c>
+      <c r="C111" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B112" t="s">
+        <v>30</v>
+      </c>
+      <c r="C112" t="e">
+        <f t="shared" ref="C112:C121" si="2">na</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B113" t="s">
+        <v>132</v>
+      </c>
+      <c r="C113" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B114" t="s">
+        <v>37</v>
+      </c>
+      <c r="C114" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B115" t="s">
+        <v>153</v>
+      </c>
+      <c r="C115" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B116" t="s">
+        <v>22</v>
+      </c>
+      <c r="C116" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B117" t="s">
+        <v>343</v>
+      </c>
+      <c r="C117" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B118" t="s">
+        <v>154</v>
+      </c>
+      <c r="C118" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B119" t="s">
+        <v>26</v>
+      </c>
+      <c r="C119" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B120" t="s">
+        <v>28</v>
+      </c>
+      <c r="C120" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="B121" t="s">
+        <v>344</v>
+      </c>
+      <c r="C121" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21E60403-B5D2-4EA3-8F86-A674DBAB247F}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8221,31 +10071,31 @@
         <v>77</v>
       </c>
       <c r="E8">
-        <f>(E6-D6*(D2/E2))/(E10/E2)</f>
+        <f t="shared" ref="E8:K8" si="0">(E6-D6*(D2/E2))/(E10/E2)</f>
         <v>3.8066666666666666</v>
       </c>
       <c r="F8">
-        <f>(F6-E6*(E2/F2))/(F10/F2)</f>
+        <f t="shared" si="0"/>
         <v>3.82</v>
       </c>
       <c r="G8">
-        <f>(G6-F6*(F2/G2))/(G10/G2)</f>
+        <f t="shared" si="0"/>
         <v>3.7939999999999996</v>
       </c>
       <c r="H8">
-        <f>(H6-G6*(G2/H2))/(H10/H2)</f>
+        <f t="shared" si="0"/>
         <v>3.8517777777777775</v>
       </c>
       <c r="I8">
-        <f>(I6-H6*(H2/I2))/(I10/I2)</f>
+        <f t="shared" si="0"/>
         <v>3.82</v>
       </c>
       <c r="J8">
-        <f>(J6-I6*(I2/J2))/(J10/J2)</f>
+        <f t="shared" si="0"/>
         <v>3.5560000000000014</v>
       </c>
       <c r="K8">
-        <f>(K6-J6*(J2/K2))/(K10/K2)</f>
+        <f t="shared" si="0"/>
         <v>3.92263157894737</v>
       </c>
       <c r="M8">
@@ -8253,23 +10103,23 @@
         <v>3.787244897959182</v>
       </c>
       <c r="N8">
-        <f t="shared" ref="L8:S8" si="0">(N6-M6*(M2/N2))/(N10/N2)</f>
+        <f t="shared" ref="N8:R8" si="1">(N6-M6*(M2/N2))/(N10/N2)</f>
         <v>3.8200000000000016</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.7584848484848496</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.81</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.5828124999999966</v>
       </c>
       <c r="R8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.8000000000000043</v>
       </c>
       <c r="S8">
@@ -8290,23 +10140,23 @@
         <v>518</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:S9" si="1">(G7-F7*(F2/G2))/(G10/G2)</f>
+        <f t="shared" ref="G9:S9" si="2">(G7-F7*(F2/G2))/(G10/G2)</f>
         <v>517.66000000000008</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>516.2466666666669</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>517.58484848484818</v>
       </c>
       <c r="J9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>512.81200000000024</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>519.77684210526331</v>
       </c>
       <c r="M9">
@@ -8314,27 +10164,27 @@
         <v>515.29122448979558</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>516.72373626373667</v>
       </c>
       <c r="O9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>516.38484848484836</v>
       </c>
       <c r="P9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>518.51627906976773</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>501.19687499999912</v>
       </c>
       <c r="R9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>513.55636363636518</v>
       </c>
       <c r="S9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>514.77457627118599</v>
       </c>
     </row>
@@ -8347,31 +10197,31 @@
         <v>33</v>
       </c>
       <c r="F10">
-        <f t="shared" ref="F10:S10" si="2">F2-E2</f>
+        <f t="shared" ref="F10:R10" si="3">F2-E2</f>
         <v>44</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>66</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>81</v>
       </c>
       <c r="M10">
@@ -8379,23 +10229,23 @@
         <v>98</v>
       </c>
       <c r="N10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>99</v>
       </c>
       <c r="P10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="R10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="S10">
@@ -8416,23 +10266,23 @@
         <v>147</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:S11" si="3">ABS(G4-F4)</f>
+        <f t="shared" ref="G11:R11" si="4">ABS(G4-F4)</f>
         <v>17</v>
       </c>
       <c r="H11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>228</v>
       </c>
       <c r="I11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="K11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="M11">
@@ -8440,23 +10290,23 @@
         <v>68</v>
       </c>
       <c r="N11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="P11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>29</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="R11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Table B8 data and Analysis
</commit_message>
<xml_diff>
--- a/fencer data/fencer_cycle_info.xlsx
+++ b/fencer data/fencer_cycle_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Python Analysis\fencer data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69896624-1E82-4F49-805F-8C7275E51FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BCE655-FC9C-4D91-9CFC-8EC44E91F850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CD2684FF-1585-4EFB-A284-DAE4AEFE2B64}"/>
+    <workbookView xWindow="-28920" yWindow="6075" windowWidth="29040" windowHeight="16440" xr2:uid="{CD2684FF-1585-4EFB-A284-DAE4AEFE2B64}"/>
   </bookViews>
   <sheets>
     <sheet name="Cycle_2020-2021" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="376">
   <si>
     <t>date</t>
   </si>
@@ -1627,9 +1627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06EEAE5-8E4F-44AE-BEEA-E9EE9F578FAC}">
   <dimension ref="A1:T168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S143" sqref="S143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7396,17 +7396,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9618D1-8B78-478F-AB82-0C3782384149}">
-  <dimension ref="A1:T73"/>
+  <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K51" sqref="K51"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.5703125" customWidth="1"/>
@@ -9244,6 +9244,304 @@
         <v>#N/A</v>
       </c>
       <c r="E73" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C74">
+        <v>1762</v>
+      </c>
+      <c r="D74" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E74" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D75" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E75" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B76" t="s">
+        <v>104</v>
+      </c>
+      <c r="C76" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D76" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E76" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B77" t="s">
+        <v>32</v>
+      </c>
+      <c r="C77" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D77" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E77" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B78" t="s">
+        <v>267</v>
+      </c>
+      <c r="C78" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D78" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E78" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B79" t="s">
+        <v>30</v>
+      </c>
+      <c r="C79" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D79" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E79" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B80" t="s">
+        <v>132</v>
+      </c>
+      <c r="C80" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D80" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E80" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B81" t="s">
+        <v>37</v>
+      </c>
+      <c r="C81">
+        <v>201</v>
+      </c>
+      <c r="D81" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E81" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B82" t="s">
+        <v>153</v>
+      </c>
+      <c r="C82" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D82" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E82" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B83" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D83" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E83" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B84" t="s">
+        <v>343</v>
+      </c>
+      <c r="C84" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D84" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E84" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B85" t="s">
+        <v>154</v>
+      </c>
+      <c r="C85" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D85" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E85" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B86" t="s">
+        <v>26</v>
+      </c>
+      <c r="C86" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D86" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E86" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C87" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D87" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E87" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>44542</v>
+      </c>
+      <c r="B88" t="s">
+        <v>344</v>
+      </c>
+      <c r="C88" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D88" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E88" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>

</xml_diff>

<commit_message>
New AAMC Data Analysis
</commit_message>
<xml_diff>
--- a/fencer data/fencer_cycle_info.xlsx
+++ b/fencer data/fencer_cycle_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TooFastDan\Documents\MD_PhD Application\Python Analysis\fencer data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE569DB-1032-4FEA-9FFE-6AE61A3C0BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448DA77D-1576-49DE-B017-0F1213E6D14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="6075" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{CD2684FF-1585-4EFB-A284-DAE4AEFE2B64}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="376">
   <si>
     <t>date</t>
   </si>
@@ -7396,11 +7396,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9618D1-8B78-478F-AB82-0C3782384149}">
-  <dimension ref="A1:T103"/>
+  <dimension ref="A1:T133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J89" sqref="J89"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H132" sqref="H132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9839,6 +9839,576 @@
         <v>#N/A</v>
       </c>
       <c r="E103" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104">
+        <v>1765</v>
+      </c>
+      <c r="D104">
+        <v>3.69</v>
+      </c>
+      <c r="E104">
+        <v>511.4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B105" t="s">
+        <v>34</v>
+      </c>
+      <c r="C105" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D105" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E105" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B106" t="s">
+        <v>104</v>
+      </c>
+      <c r="C106" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D106" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E106" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B107" t="s">
+        <v>32</v>
+      </c>
+      <c r="C107" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D107" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E107" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B108" t="s">
+        <v>267</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>4</v>
+      </c>
+      <c r="E108">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B109" t="s">
+        <v>30</v>
+      </c>
+      <c r="C109" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D109" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E109" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B110" t="s">
+        <v>132</v>
+      </c>
+      <c r="C110" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D110" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E110" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B111" t="s">
+        <v>37</v>
+      </c>
+      <c r="C111">
+        <v>338</v>
+      </c>
+      <c r="D111">
+        <v>517.5</v>
+      </c>
+      <c r="E111">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B112" t="s">
+        <v>153</v>
+      </c>
+      <c r="C112" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D112" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E112" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B113" t="s">
+        <v>22</v>
+      </c>
+      <c r="C113" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D113" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E113" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B114" t="s">
+        <v>343</v>
+      </c>
+      <c r="C114" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D114" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E114" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B115" t="s">
+        <v>154</v>
+      </c>
+      <c r="C115" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D115" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E115" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B116" t="s">
+        <v>26</v>
+      </c>
+      <c r="C116" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D116" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E116" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B117" t="s">
+        <v>28</v>
+      </c>
+      <c r="C117" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D117" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E117" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>44566</v>
+      </c>
+      <c r="B118" t="s">
+        <v>344</v>
+      </c>
+      <c r="C118" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D118" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E118" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B119" t="s">
+        <v>33</v>
+      </c>
+      <c r="C119">
+        <v>1766</v>
+      </c>
+      <c r="D119">
+        <v>3.69</v>
+      </c>
+      <c r="E119">
+        <v>511.4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B120" t="s">
+        <v>34</v>
+      </c>
+      <c r="C120">
+        <v>40</v>
+      </c>
+      <c r="D120">
+        <v>3.73</v>
+      </c>
+      <c r="E120">
+        <v>512.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B121" t="s">
+        <v>104</v>
+      </c>
+      <c r="C121">
+        <v>1051</v>
+      </c>
+      <c r="D121">
+        <v>3.65</v>
+      </c>
+      <c r="E121">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B122" t="s">
+        <v>32</v>
+      </c>
+      <c r="C122" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D122" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E122" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B123" t="s">
+        <v>267</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
+      <c r="D123">
+        <v>3.99</v>
+      </c>
+      <c r="E123">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B124" t="s">
+        <v>30</v>
+      </c>
+      <c r="C124" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D124" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E124" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B125" t="s">
+        <v>132</v>
+      </c>
+      <c r="C125" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D125" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E125" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B126" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126">
+        <v>378</v>
+      </c>
+      <c r="D126">
+        <v>3.84</v>
+      </c>
+      <c r="E126">
+        <v>517.4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B127" t="s">
+        <v>153</v>
+      </c>
+      <c r="C127">
+        <v>165</v>
+      </c>
+      <c r="D127">
+        <v>3.67</v>
+      </c>
+      <c r="E127">
+        <v>511.4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B128" t="s">
+        <v>22</v>
+      </c>
+      <c r="C128" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D128" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E128" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B129" t="s">
+        <v>343</v>
+      </c>
+      <c r="C129" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D129" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E129" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B130" t="s">
+        <v>154</v>
+      </c>
+      <c r="C130">
+        <v>132</v>
+      </c>
+      <c r="D130">
+        <v>3.58</v>
+      </c>
+      <c r="E130">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B131" t="s">
+        <v>26</v>
+      </c>
+      <c r="C131" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D131" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E131" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B132" t="s">
+        <v>28</v>
+      </c>
+      <c r="C132" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D132" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E132" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>44576</v>
+      </c>
+      <c r="B133" t="s">
+        <v>344</v>
+      </c>
+      <c r="C133" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D133" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E133" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>

</xml_diff>